<commit_message>
update png and excel.
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenton\OneDrive\_SYNC\University - 3\Math3202\math3202\assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BBCA2B-E042-486F-90B6-6FF9411BDA25}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{3340550B-59B5-453C-A3FD-FFD2A21870B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B0A0E779-BA5C-4C1B-B6EB-89C18BB42920}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="6293" xr2:uid="{0949A393-2346-431C-A120-94B7CF561785}"/>
   </bookViews>
@@ -136,7 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -170,6 +170,9 @@
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -488,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93FC566C-F5D9-4113-AD03-15D1C2A9B76C}">
   <dimension ref="B2:N12"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="166" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="21.4" x14ac:dyDescent="0.45"/>
@@ -502,7 +505,7 @@
     <col min="7" max="7" width="17.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="2.59765625" style="1" customWidth="1"/>
     <col min="9" max="9" width="3.59765625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="17.796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.53125" style="1" customWidth="1"/>
     <col min="11" max="11" width="12.73046875" style="1"/>
     <col min="12" max="12" width="13.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.73046875" style="1"/>
@@ -537,13 +540,13 @@
       <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="12">
         <v>140776</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="12">
         <v>3276000</v>
       </c>
       <c r="H3" s="5"/>
@@ -629,13 +632,13 @@
       <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="12">
         <v>150128</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="12">
         <v>32461</v>
       </c>
       <c r="H6" s="5" t="s">
@@ -671,13 +674,13 @@
       <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="12">
         <v>153633</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="12">
         <v>59020</v>
       </c>
       <c r="H7" s="5" t="s">
@@ -713,13 +716,13 @@
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="12">
         <v>142088</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="12">
         <v>0</v>
       </c>
       <c r="H8" s="5" t="s">
@@ -755,13 +758,13 @@
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="12">
         <v>164098</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="12">
         <v>59020</v>
       </c>
       <c r="H9" s="5" t="s">
@@ -797,13 +800,13 @@
       <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="12">
         <v>258664</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="12">
         <v>129844</v>
       </c>
       <c r="H10" s="5" t="s">

</xml_diff>